<commit_message>
Feito ajustes nos eixos e correções de dados
</commit_message>
<xml_diff>
--- a/vendas_mes.xlsx
+++ b/vendas_mes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="8640" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="8640" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas" sheetId="1" state="hidden" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
   <si>
     <t>LJ 02</t>
   </si>
@@ -90,7 +90,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -153,16 +153,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -797,21 +797,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -820,7 +820,7 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
@@ -829,7 +829,7 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
@@ -838,7 +838,7 @@
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="7">
@@ -847,7 +847,7 @@
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="7">
@@ -856,115 +856,124 @@
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B7" s="7">
         <v>230356.75</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="7">
         <v>241705.44</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B9" s="7">
         <v>338541.85</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <v>296342.18</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B11" s="7">
         <v>217601.91</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B12" s="7">
         <v>600505.37</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="7">
         <v>274684.02</v>
       </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="7">
         <v>279966.96999999997</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B15" s="7">
         <v>296041.73</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B16" s="7">
         <v>261157.32</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B17" s="7">
         <v>312801.94</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B18" s="7">
         <v>3467.79</v>
       </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -973,20 +982,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -994,135 +1003,143 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>198057.85</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>297737.39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>358489.41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>252240.3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B7" s="7">
         <v>235597.9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B8" s="7">
         <v>240277.58</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="7">
         <v>524183.82</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B10" s="7">
         <v>307361.46999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B11" s="7">
         <v>256261.51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B12" s="7">
         <v>635547.72</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B13" s="7">
         <v>307233.90999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B14" s="7">
         <v>331246.2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B15" s="7">
         <v>332227.89</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B16" s="7">
         <v>319662.14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B17" s="7">
         <v>393355.13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B18" s="7">
         <v>2800.93</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1133,156 +1150,161 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
         <v>214252.46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="7">
         <v>306813</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
         <v>343383.71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="7">
         <v>222742.2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
         <v>50209.49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
         <v>200595.74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="7">
         <v>185421.42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="7">
         <v>308910.23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="7">
         <v>330590.23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="7">
         <v>246054.86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="7">
         <v>652885.47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="7">
         <v>288292.31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="7">
         <v>321289.38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="7">
         <v>310239.95</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="7">
         <v>240636.68</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="7">
         <v>355967.87</v>
       </c>
-      <c r="G17" s="11"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="11"/>
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>